<commit_message>
Updating staff/teacher population ratios
</commit_message>
<xml_diff>
--- a/data/raw/cost_ratio.xlsx
+++ b/data/raw/cost_ratio.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://validuseconomicscom.sharepoint.com/sites/WaapihkResearch/Shared Documents/General/Client &amp; Project Folders/AMC/Education/REA/Enhancements/Remoteness/Nishnawbe Aski Nation Remoteness Approach for AMC/sources/R/nan_remoteness/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{CB8DEAB7-3DF9-9746-8B25-9CD2C50D58FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C612FE21-806C-1645-AFE3-09176A50067C}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{CB8DEAB7-3DF9-9746-8B25-9CD2C50D58FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F166F2A0-168F-984D-8B11-21DA8AB10BB7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{5D26BE13-762D-7549-9210-AEBBEDE27BC4}"/>
+    <workbookView xWindow="39960" yWindow="-21100" windowWidth="28800" windowHeight="17500" xr2:uid="{5D26BE13-762D-7549-9210-AEBBEDE27BC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>FTE row</t>
-  </si>
-  <si>
-    <t>Non-FTE row</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Pinaymootang</t>
   </si>
@@ -78,6 +72,18 @@
   </si>
   <si>
     <t>First Nation</t>
+  </si>
+  <si>
+    <t>Non-FTE with per capita</t>
+  </si>
+  <si>
+    <t>Non-FTE no per capita</t>
+  </si>
+  <si>
+    <t>FTE no per capita</t>
+  </si>
+  <si>
+    <t>FTE with per capita</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7825D652-8279-9245-8ADB-CB4F1537D3DB}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,22 +446,29 @@
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="26.83203125" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2">
         <v>0.56387856999999997</v>
@@ -463,10 +476,16 @@
       <c r="C2">
         <v>1.773431467</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0.642411446</v>
+      </c>
+      <c r="E2">
+        <v>1.55663478</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0.57989203499999997</v>
@@ -474,10 +493,16 @@
       <c r="C3">
         <v>1.7244589320000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0.71030933200000002</v>
+      </c>
+      <c r="E3">
+        <v>1.407837338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1.0426098150000001</v>
@@ -485,10 +510,16 @@
       <c r="C4">
         <v>0.95913158099999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>1.014542327</v>
+      </c>
+      <c r="E4">
+        <v>0.98566612099999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0.97710522499999997</v>
@@ -496,10 +527,16 @@
       <c r="C5">
         <v>1.0234312270000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>1.0478952340000001</v>
+      </c>
+      <c r="E5">
+        <v>0.95429387099999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0.52603019799999995</v>
@@ -507,10 +544,16 @@
       <c r="C6">
         <v>1.9010315449999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0.68469064300000004</v>
+      </c>
+      <c r="E6">
+        <v>1.460513605</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1.7241485919999999</v>
@@ -518,10 +561,16 @@
       <c r="C7">
         <v>0.57999641400000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>2.1866640180000001</v>
+      </c>
+      <c r="E7">
+        <v>0.457317627</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>0.76448750799999998</v>
@@ -529,10 +578,16 @@
       <c r="C8">
         <v>1.3080658469999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>1.1474320600000001</v>
+      </c>
+      <c r="E8">
+        <v>0.87151129400000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0.75905266000000005</v>
@@ -540,10 +595,16 @@
       <c r="C9">
         <v>1.3174316530000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>1.0355111560000001</v>
+      </c>
+      <c r="E9">
+        <v>0.96570664100000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1.0143591540000001</v>
@@ -551,10 +612,16 @@
       <c r="C10">
         <v>0.98584411299999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>1.2974916400000001</v>
+      </c>
+      <c r="E10">
+        <v>0.770717875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2.4225438349999999</v>
@@ -562,10 +629,16 @@
       <c r="C11">
         <v>0.41278922800000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>2.5637534290000001</v>
+      </c>
+      <c r="E11">
+        <v>0.39005311100000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0.91574070799999996</v>
@@ -573,10 +646,16 @@
       <c r="C12">
         <v>1.092012172</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>1.256826921</v>
+      </c>
+      <c r="E12">
+        <v>0.79565450299999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -585,6 +664,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="bfb77542-f000-416e-9391-d4f3ed66f756" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b313e45-d48c-4d36-b475-2ce2b8c74c54">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0E76F91975C3B469A9C9E5B90195820" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d044a0b9c54eefe6672bdcd1de2a28d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b313e45-d48c-4d36-b475-2ce2b8c74c54" xmlns:ns3="bfb77542-f000-416e-9391-d4f3ed66f756" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d9534cf13e5bbdf06d33948ab5fbaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="2b313e45-d48c-4d36-b475-2ce2b8c74c54"/>
@@ -827,7 +917,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -836,25 +926,46 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="bfb77542-f000-416e-9391-d4f3ed66f756" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b313e45-d48c-4d36-b475-2ce2b8c74c54">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58FC9ED7-BF3A-4589-BB6A-33422F1EA2A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="bfb77542-f000-416e-9391-d4f3ed66f756"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2b313e45-d48c-4d36-b475-2ce2b8c74c54"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{184554EA-65AD-460B-90AC-99E2F9665B5C}"/>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{184554EA-65AD-460B-90AC-99E2F9665B5C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b313e45-d48c-4d36-b475-2ce2b8c74c54"/>
+    <ds:schemaRef ds:uri="bfb77542-f000-416e-9391-d4f3ed66f756"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FC3C239-3B7E-4C71-AF3B-16408E3636C4}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58FC9ED7-BF3A-4589-BB6A-33422F1EA2A7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FC3C239-3B7E-4C71-AF3B-16408E3636C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>